<commit_message>
Add trimming leading/trailing white spaces in ID
</commit_message>
<xml_diff>
--- a/tests/test_empleados_bac.xlsx
+++ b/tests/test_empleados_bac.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -46,10 +46,13 @@
     <t xml:space="preserve">Def</t>
   </si>
   <si>
-    <t xml:space="preserve">IJK LMN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ijk</t>
+    <t xml:space="preserve">01 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID con apostrofe y espacio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPQ</t>
   </si>
 </sst>
 </file>
@@ -60,7 +63,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="00000000000000"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -81,13 +84,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -132,20 +128,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -166,13 +158,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.91"/>
@@ -193,13 +185,13 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="0" t="n">
         <v>123</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="C2" s="1" t="n">
         <v>789</v>
       </c>
       <c r="D2" s="0" t="s">
@@ -207,157 +199,152 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+      <c r="A3" s="0" t="n">
         <v>987654321</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="n">
+      <c r="C3" s="1" t="n">
         <v>123</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
-        <v>55544433</v>
-      </c>
-      <c r="B4" s="2" t="s">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="2" t="n">
-        <v>456</v>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>321</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="A9" s="2"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
+      <c r="A11" s="2"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="A12" s="2"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
+      <c r="A13" s="2"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+      <c r="A14" s="2"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+      <c r="A16" s="2"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
+      <c r="A17" s="2"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
+      <c r="A19" s="2"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="A20" s="2"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
+      <c r="A21" s="2"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
+      <c r="A22" s="2"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
+      <c r="A23" s="2"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
+      <c r="A24" s="2"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
+      <c r="A25" s="2"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
+      <c r="A26" s="2"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
+      <c r="A27" s="2"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
+      <c r="A28" s="2"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>